<commit_message>
added an eight starred sample
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomto\Desktop\FINAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AD4871-AB00-4EB5-96F0-08258134A204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA60BC04-33C0-45A0-B8FB-3821B8ADBA10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{73AD2DE4-4563-4805-96BF-3FF488B20A72}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4200" uniqueCount="1445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4201" uniqueCount="1446">
   <si>
     <t>TJC L alexander</t>
   </si>
@@ -4906,6 +4906,9 @@
   </si>
   <si>
     <t>image03147</t>
+  </si>
+  <si>
+    <t>10483704s</t>
   </si>
 </sst>
 </file>
@@ -4991,7 +4994,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5015,8 +5018,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -25063,23 +25065,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA06A63-AD4C-4BF6-9307-18280840F412}">
-  <dimension ref="A1:B293"/>
+  <dimension ref="A1:B294"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.28515625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="11" t="s">
         <v>1431</v>
       </c>
     </row>
@@ -25108,10 +25110,10 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>1437</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>0</v>
       </c>
     </row>
@@ -27324,98 +27326,106 @@
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="12" t="s">
+      <c r="A282" s="11" t="s">
         <v>1432</v>
       </c>
-      <c r="B282" s="12">
+      <c r="B282" s="11">
         <v>8</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="12" t="s">
+      <c r="A283" s="11" t="s">
         <v>1433</v>
       </c>
-      <c r="B283" s="12">
+      <c r="B283" s="11">
         <v>8</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="12" t="s">
+      <c r="A284" s="11" t="s">
         <v>1434</v>
       </c>
-      <c r="B284" s="12">
+      <c r="B284" s="11">
         <v>8</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="12" t="s">
+      <c r="A285" s="11" t="s">
         <v>1435</v>
       </c>
-      <c r="B285" s="12">
+      <c r="B285" s="11">
         <v>8</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="12" t="s">
+      <c r="A286" s="11" t="s">
         <v>1436</v>
       </c>
-      <c r="B286" s="12">
+      <c r="B286" s="11">
         <v>8</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="12" t="s">
+      <c r="A287" s="11" t="s">
         <v>1438</v>
       </c>
-      <c r="B287" s="12">
+      <c r="B287" s="11">
         <v>8</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="12" t="s">
+      <c r="A288" s="11" t="s">
         <v>1439</v>
       </c>
-      <c r="B288" s="12">
+      <c r="B288" s="11">
         <v>8</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="12" t="s">
+      <c r="A289" s="11" t="s">
         <v>1440</v>
       </c>
-      <c r="B289" s="12">
+      <c r="B289" s="11">
         <v>8</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="12" t="s">
+      <c r="A290" s="11" t="s">
         <v>1441</v>
       </c>
-      <c r="B290" s="12">
+      <c r="B290" s="11">
         <v>8</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" s="12" t="s">
+      <c r="A291" s="11" t="s">
         <v>1442</v>
       </c>
-      <c r="B291" s="12">
+      <c r="B291" s="11">
         <v>8</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" s="12" t="s">
+      <c r="A292" s="11" t="s">
         <v>1443</v>
       </c>
-      <c r="B292" s="12">
+      <c r="B292" s="11">
         <v>8</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="12" t="s">
+      <c r="A293" s="11" t="s">
         <v>1444</v>
       </c>
-      <c r="B293" s="12">
+      <c r="B293" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" s="11" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B294" s="11">
         <v>8</v>
       </c>
     </row>

</xml_diff>